<commit_message>
fix the wires around MAX31855
</commit_message>
<xml_diff>
--- a/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer_bom.xlsx
+++ b/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitanoitaru/Desktop/M1/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FC4800-39A6-A141-9651-65217E7610E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B9C273-50CB-2C44-B9E7-025D3F9AE54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CoolingBoxWireOrganizer_bom" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="153">
   <si>
     <t>Reference</t>
   </si>
@@ -561,6 +561,25 @@
   <si>
     <t>connector of thermocouple</t>
     <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>型番</t>
+    <rPh sb="0" eb="2">
+      <t>カタバn</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>KGF15AR71E104KT</t>
+  </si>
+  <si>
+    <t>GCM188R71H103KA37J</t>
+  </si>
+  <si>
+    <t>CDBU0245</t>
+  </si>
+  <si>
+    <t>501331-0407</t>
   </si>
 </sst>
 </file>
@@ -1548,21 +1567,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="33.42578125" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.28515625" customWidth="1"/>
+    <col min="6" max="7" width="38.85546875" customWidth="1"/>
+    <col min="8" max="8" width="78.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1582,10 +1601,13 @@
         <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1605,10 +1627,13 @@
         <v>56</v>
       </c>
       <c r="G2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1628,10 +1653,13 @@
         <v>56</v>
       </c>
       <c r="G3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1651,10 +1679,13 @@
         <v>57</v>
       </c>
       <c r="G4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1674,10 +1705,13 @@
         <v>58</v>
       </c>
       <c r="G5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -1696,11 +1730,11 @@
       <c r="F6" t="s">
         <v>62</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1719,11 +1753,11 @@
       <c r="F7" t="s">
         <v>67</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1742,11 +1776,11 @@
       <c r="F8" t="s">
         <v>71</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1765,11 +1799,11 @@
       <c r="F9" t="s">
         <v>111</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -1788,11 +1822,11 @@
       <c r="F10" t="s">
         <v>77</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1811,11 +1845,11 @@
       <c r="F11" t="s">
         <v>115</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1834,11 +1868,11 @@
       <c r="F12" t="s">
         <v>81</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1857,11 +1891,11 @@
       <c r="F13" t="s">
         <v>121</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1880,11 +1914,11 @@
       <c r="F14" t="s">
         <v>94</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1903,11 +1937,12 @@
       <c r="F15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="3"/>
+      <c r="H15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1926,11 +1961,12 @@
       <c r="F16" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="3"/>
+      <c r="H16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1949,11 +1985,12 @@
       <c r="F17" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="3"/>
+      <c r="H17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1972,11 +2009,12 @@
       <c r="F18" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="3"/>
+      <c r="H18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1995,11 +2033,11 @@
       <c r="F19" t="s">
         <v>92</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -2019,7 +2057,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -2039,7 +2077,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="C24" s="2" t="s">
         <v>59</v>
       </c>
@@ -2053,7 +2091,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="C25" s="2" t="s">
         <v>64</v>
       </c>
@@ -2067,7 +2105,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="C26" s="2" t="s">
         <v>74</v>
       </c>
@@ -2081,7 +2119,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="C27" s="2" t="s">
         <v>79</v>
       </c>
@@ -2095,7 +2133,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="C28" s="2" t="s">
         <v>89</v>
       </c>
@@ -2109,7 +2147,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="C29" s="2" t="s">
         <v>132</v>
       </c>
@@ -2123,7 +2161,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="C30" s="2" t="s">
         <v>135</v>
       </c>
@@ -2137,7 +2175,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="C32" t="s">
         <v>124</v>
       </c>
@@ -2151,7 +2189,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="3:7">
+    <row r="33" spans="3:8">
       <c r="C33" t="s">
         <v>140</v>
       </c>
@@ -2164,11 +2202,11 @@
       <c r="F33" t="s">
         <v>120</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="3:7">
+    <row r="35" spans="3:8">
       <c r="D35">
         <v>4</v>
       </c>
@@ -2178,11 +2216,11 @@
       <c r="F35" t="s">
         <v>122</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="3:7">
+    <row r="36" spans="3:8">
       <c r="D36">
         <v>1</v>
       </c>
@@ -2193,7 +2231,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="3:7">
+    <row r="37" spans="3:8">
       <c r="D37">
         <v>4</v>
       </c>
@@ -2204,7 +2242,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="3:7">
+    <row r="39" spans="3:8">
       <c r="C39" s="2" t="s">
         <v>142</v>
       </c>

</xml_diff>

<commit_message>
add peltier power relay socket to bom
</commit_message>
<xml_diff>
--- a/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer_bom.xlsx
+++ b/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitanoitaru/Desktop/M1/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E684938-E665-364B-9380-BCFF2A0D4953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80B1887-8D44-CB48-99A6-0CF998E1C38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CoolingBoxWireOrganizer_bom" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="187">
   <si>
     <t>Reference</t>
   </si>
@@ -701,6 +701,16 @@
       <t>ゴウケイ</t>
     </rPh>
     <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>peltier power relay DIN rail socket</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P2RFZ-05-E</t>
+  </si>
+  <si>
+    <t>https://www.monotaro.com/p/5059/4050/?t.q=p2rfz-05-e</t>
   </si>
 </sst>
 </file>
@@ -1697,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1803,7 +1813,7 @@
         <v>26</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I40" si="0">D3*H3</f>
+        <f t="shared" ref="I3:I41" si="0">D3*H3</f>
         <v>104</v>
       </c>
       <c r="J3" t="s">
@@ -2633,57 +2643,72 @@
       </c>
     </row>
     <row r="34" spans="3:9">
-      <c r="C34" s="2" t="s">
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F34" t="s">
+        <v>184</v>
+      </c>
+      <c r="G34" t="s">
+        <v>185</v>
+      </c>
+      <c r="H34">
+        <v>479</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>958</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9">
+      <c r="C35" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F34" t="s">
-        <v>162</v>
-      </c>
-      <c r="G34" t="s">
-        <v>170</v>
-      </c>
-      <c r="H34">
-        <v>2581</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="0"/>
-        <v>2581</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9">
-      <c r="C35" t="s">
-        <v>172</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" t="s">
+        <v>170</v>
+      </c>
+      <c r="H35">
+        <v>2581</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9">
+      <c r="C36" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>174</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>173</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <v>1838</v>
       </c>
-      <c r="I35">
+      <c r="I36">
         <f t="shared" si="0"/>
         <v>1838</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9">
-      <c r="I36">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="37" spans="3:9">
@@ -2699,57 +2724,63 @@
       </c>
     </row>
     <row r="39" spans="3:9">
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>182</v>
-      </c>
-      <c r="F39" t="s">
-        <v>180</v>
-      </c>
-      <c r="G39" t="s">
-        <v>181</v>
-      </c>
-      <c r="H39">
-        <v>7445</v>
-      </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>7445</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="3:9">
-      <c r="C40" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="D40">
         <v>1</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" t="s">
+        <v>182</v>
+      </c>
+      <c r="F40" t="s">
+        <v>180</v>
+      </c>
+      <c r="G40" t="s">
+        <v>181</v>
+      </c>
+      <c r="H40">
+        <v>7445</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>7445</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9">
+      <c r="C41" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>127</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G41" t="s">
         <v>175</v>
       </c>
-      <c r="H40">
+      <c r="H41">
         <v>3841</v>
       </c>
-      <c r="I40">
+      <c r="I41">
         <f t="shared" si="0"/>
         <v>3841</v>
       </c>
     </row>
-    <row r="41" spans="3:9">
-      <c r="H41" s="4" t="s">
+    <row r="42" spans="3:9">
+      <c r="H42" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="I41" s="4">
-        <f>SUM(I2:I40)</f>
-        <v>43067</v>
+      <c r="I42" s="4">
+        <f>SUM(I2:I41)</f>
+        <v>44025</v>
       </c>
     </row>
   </sheetData>
@@ -2793,18 +2824,18 @@
     <hyperlink ref="E33" r:id="rId36" xr:uid="{CDD17023-1799-5447-8B56-11DB914F137F}"/>
     <hyperlink ref="E25" r:id="rId37" xr:uid="{B647E682-FCD9-5C45-B340-639370BCF843}"/>
     <hyperlink ref="E24" r:id="rId38" xr:uid="{AF0CF161-773B-624A-9BC8-A2E937BD8AF4}"/>
-    <hyperlink ref="C40" r:id="rId39" xr:uid="{5C34EE02-39EE-DA4C-99FF-8856F5801811}"/>
-    <hyperlink ref="E40" r:id="rId40" xr:uid="{18855DE2-69F4-2E4C-9C9C-16F5B0E96D39}"/>
+    <hyperlink ref="C41" r:id="rId39" xr:uid="{5C34EE02-39EE-DA4C-99FF-8856F5801811}"/>
+    <hyperlink ref="E41" r:id="rId40" xr:uid="{18855DE2-69F4-2E4C-9C9C-16F5B0E96D39}"/>
     <hyperlink ref="E11" r:id="rId41" xr:uid="{57FA8A9A-01C3-9448-892F-3FCFB5997974}"/>
     <hyperlink ref="E13" r:id="rId42" xr:uid="{5D69BCAD-740D-3F4E-AC72-EDD047C0C10D}"/>
     <hyperlink ref="E16" r:id="rId43" xr:uid="{FCA28E44-1755-144A-8455-BFE649F6B676}"/>
     <hyperlink ref="E18" r:id="rId44" xr:uid="{D08D1D80-E223-F949-B0E8-823CB2A1D13C}"/>
     <hyperlink ref="E29" r:id="rId45" xr:uid="{13EF6D69-42D3-A640-863F-16CB3B715AAB}"/>
     <hyperlink ref="E30" r:id="rId46" xr:uid="{383096AE-AF3B-A846-A184-7889A98C959F}"/>
-    <hyperlink ref="C34" r:id="rId47" xr:uid="{5F946CBC-3488-834C-A9A6-AD5B3C9F7E94}"/>
+    <hyperlink ref="C35" r:id="rId47" xr:uid="{5F946CBC-3488-834C-A9A6-AD5B3C9F7E94}"/>
     <hyperlink ref="E32" r:id="rId48" xr:uid="{9EE2766B-5521-F343-B843-556524BC0A2A}"/>
-    <hyperlink ref="E34" r:id="rId49" xr:uid="{6530E51E-7AAB-3B4D-A42C-69172B8BC0B9}"/>
-    <hyperlink ref="E35" r:id="rId50" xr:uid="{0EFE1CFD-3899-4545-95EB-5F532D993A0E}"/>
+    <hyperlink ref="E35" r:id="rId49" xr:uid="{6530E51E-7AAB-3B4D-A42C-69172B8BC0B9}"/>
+    <hyperlink ref="E36" r:id="rId50" xr:uid="{0EFE1CFD-3899-4545-95EB-5F532D993A0E}"/>
     <hyperlink ref="C29" r:id="rId51" xr:uid="{DBB7A5C1-EFCA-7C4E-93EA-841FA1D2CCEA}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add information of terminal block and what is used at Kyushu site
</commit_message>
<xml_diff>
--- a/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer_bom.xlsx
+++ b/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitanoitaru/Desktop/M1/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F19E61-5CD6-E541-9C84-D3925C502894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C844AFB9-138D-CD44-BCDC-5169454237BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="1340" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CoolingBoxWireOrganizer_bom" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="209">
   <si>
     <t>Reference</t>
   </si>
@@ -712,6 +712,76 @@
   <si>
     <t>MDR-60-12</t>
     <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>terminal block</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>https://www.digikey.jp/ja/products/detail/phoenix-contact/3273198/7596982</t>
+  </si>
+  <si>
+    <t>https://www.phoenixcontact.com/en-us/products/distributor-terminal-block-ptfix-66x25-ns35a-gy-3273198?type=pdf</t>
+  </si>
+  <si>
+    <t>power cord splicing</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>https://www.digikey.jp/ja/products/detail/phoenix-contact/3210499/2263754</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/388/3210499.pdf</t>
+  </si>
+  <si>
+    <t>Circuit Base Pillar </t>
+  </si>
+  <si>
+    <t>F25L-415.0-2-U </t>
+  </si>
+  <si>
+    <t>740/m</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>鉄後入れTロック25 </t>
+  </si>
+  <si>
+    <t>TL2X </t>
+  </si>
+  <si>
+    <t>https://www.yukilabo.co.jp/index.php?LECOFRAME</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>テーパーボルト25 </t>
+  </si>
+  <si>
+    <t>Fナット25 </t>
+  </si>
+  <si>
+    <t>TB25 </t>
+  </si>
+  <si>
+    <t>NF25-M4 </t>
+  </si>
+  <si>
+    <t>アルミ(A5052)切板 厚さ3mm(Front Panel)</t>
+  </si>
+  <si>
+    <t>配線ダクト</t>
+  </si>
+  <si>
+    <t>DINレール</t>
+  </si>
+  <si>
+    <t>https://www.monotaro.com/p/0964/9981/?t.q=9649981</t>
+  </si>
+  <si>
+    <t>https://www.monotaro.com/p/3710/8881/?t.q=37108881</t>
+  </si>
+  <si>
+    <t>https://www.monotaro.com/p/6729/8762/?t.q=67298762</t>
   </si>
 </sst>
 </file>
@@ -1336,7 +1406,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1351,6 +1421,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1708,10 +1787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="E44" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1814,7 +1893,7 @@
         <v>26</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I41" si="0">D3*H3</f>
+        <f t="shared" ref="I3:I48" si="0">D3*H3</f>
         <v>104</v>
       </c>
       <c r="J3" t="s">
@@ -2776,15 +2855,231 @@
       </c>
     </row>
     <row r="42" spans="3:9">
-      <c r="H42" s="4" t="s">
+      <c r="H42" s="6"/>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9">
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9">
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9">
+      <c r="C45" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F45" t="s">
+        <v>187</v>
+      </c>
+      <c r="G45" s="5">
+        <v>3273198</v>
+      </c>
+      <c r="H45">
+        <v>656</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9">
+      <c r="C46" t="s">
+        <v>192</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>191</v>
+      </c>
+      <c r="F46" t="s">
+        <v>190</v>
+      </c>
+      <c r="G46" s="5">
+        <v>3210499</v>
+      </c>
+      <c r="H46">
+        <v>1219</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9">
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="3:9">
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9">
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F49" t="s">
+        <v>193</v>
+      </c>
+      <c r="G49" t="s">
+        <v>194</v>
+      </c>
+      <c r="H49" t="s">
+        <v>195</v>
+      </c>
+      <c r="I49">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9">
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="F50" t="s">
+        <v>196</v>
+      </c>
+      <c r="G50" t="s">
+        <v>197</v>
+      </c>
+      <c r="H50">
+        <v>110</v>
+      </c>
+      <c r="I50">
+        <f>D50*H50</f>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9">
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" t="s">
+        <v>199</v>
+      </c>
+      <c r="G51" t="s">
+        <v>201</v>
+      </c>
+      <c r="H51">
+        <v>30</v>
+      </c>
+      <c r="I51">
+        <f t="shared" ref="I51:I56" si="1">D51*H51</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9">
+      <c r="D52">
+        <v>12</v>
+      </c>
+      <c r="E52" s="7"/>
+      <c r="F52" t="s">
+        <v>200</v>
+      </c>
+      <c r="G52" t="s">
+        <v>202</v>
+      </c>
+      <c r="H52">
+        <v>32</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="53" spans="4:9">
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:9">
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>206</v>
+      </c>
+      <c r="F54" t="s">
+        <v>203</v>
+      </c>
+      <c r="H54">
+        <v>3290</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="1"/>
+        <v>3290</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9">
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>207</v>
+      </c>
+      <c r="F55" t="s">
+        <v>204</v>
+      </c>
+      <c r="H55">
+        <v>1898</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>3796</v>
+      </c>
+    </row>
+    <row r="56" spans="4:9">
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>208</v>
+      </c>
+      <c r="F56" t="s">
+        <v>205</v>
+      </c>
+      <c r="H56">
+        <v>399</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="1"/>
+        <v>798</v>
+      </c>
+    </row>
+    <row r="57" spans="4:9">
+      <c r="H57" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I42" s="4">
-        <f>SUM(I2:I41)</f>
-        <v>49796</v>
+      <c r="I57" s="4">
+        <f>SUM(I2:I56)</f>
+        <v>65024</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E49:E52"/>
+  </mergeCells>
   <phoneticPr fontId="18"/>
   <hyperlinks>
     <hyperlink ref="C19" r:id="rId1" xr:uid="{EA5F875B-1A23-3244-BF02-CEAD3D27270E}"/>
@@ -2838,6 +3133,7 @@
     <hyperlink ref="E35" r:id="rId49" xr:uid="{6530E51E-7AAB-3B4D-A42C-69172B8BC0B9}"/>
     <hyperlink ref="E36" r:id="rId50" xr:uid="{0EFE1CFD-3899-4545-95EB-5F532D993A0E}"/>
     <hyperlink ref="C29" r:id="rId51" xr:uid="{DBB7A5C1-EFCA-7C4E-93EA-841FA1D2CCEA}"/>
+    <hyperlink ref="E49" r:id="rId52" xr:uid="{4F5184F6-E1B2-804C-92DE-E2E074A050D8}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
change the format of bom(add memo)
</commit_message>
<xml_diff>
--- a/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer_bom.xlsx
+++ b/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitanoitaru/Desktop/M1/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C844AFB9-138D-CD44-BCDC-5169454237BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64573B83-580E-E448-9277-83164A84C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1340" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36420" yWindow="780" windowWidth="30780" windowHeight="21760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CoolingBoxWireOrganizer_bom" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="197">
   <si>
     <t>Reference</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Datasheet</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>0.1u</t>
   </si>
   <si>
-    <t>Capacitor_SMD:C_0603_1608Metric_Pad1.08x0.95mm_HandSolder</t>
-  </si>
-  <si>
     <t>C2,C3,C4,C5</t>
   </si>
   <si>
@@ -70,24 +64,15 @@
     <t>D</t>
   </si>
   <si>
-    <t>Diode_SMD:D_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
-  </si>
-  <si>
     <t>J1,J11,J16</t>
   </si>
   <si>
     <t>Conn_02x02_Odd_Even</t>
   </si>
   <si>
-    <t>my_expanded_footprint_library:Molex_Pico-Clasp_501331-0407_1x04-1MP_P1.00mm_Vertical</t>
-  </si>
-  <si>
     <t>Conn_01x02</t>
   </si>
   <si>
-    <t>-- 繝溘ャ繧ｯ繧ｹ縺輔ｌ縺溷､ --</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
@@ -106,9 +91,6 @@
     <t>Conn_01x08_Pin</t>
   </si>
   <si>
-    <t>Connector_PinHeader_2.54mm:PinHeader_1x08_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t>Conn_02x03_Odd_Even</t>
   </si>
   <si>
@@ -118,33 +100,21 @@
     <t>Conn_02x18_Odd_Even</t>
   </si>
   <si>
-    <t>Connector_PinHeader_2.54mm:PinHeader_2x18_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t>J18,J19,J23</t>
   </si>
   <si>
     <t>DILB16P-223TLF</t>
   </si>
   <si>
-    <t>my_library:AMPHENOL_DILB16P-223TLF</t>
-  </si>
-  <si>
     <t>L1,L2,L3,L4,L5,L6,L7,L8</t>
   </si>
   <si>
     <t>L_Ferrite</t>
   </si>
   <si>
-    <t>Inductor_SMD:L_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
-  </si>
-  <si>
     <t>R1,R12,R13,R15,R17,R19</t>
   </si>
   <si>
-    <t>Resistor_SMD:R_0603_1608Metric_Pad0.98x0.95mm_HandSolder</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -161,9 +131,6 @@
   </si>
   <si>
     <t>MAX31855KASA</t>
-  </si>
-  <si>
-    <t>my_expanded_footprint_library:SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
     <t>http://datasheets.maximintegrated.com/en/ds/MAX31855.pdf</t>
@@ -177,10 +144,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>Capacitor_SMD:C_0603_1608Metric_Pad1.08x0.95mm_HandSolder</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>https://www.mouser.jp/ProductDetail/Murata-Electronics/GCM188R71H103KA37J?qs=N3Kl9KD794T3%2FxlXdF0Axg%3D%3D</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -255,10 +218,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>my_expanded_footprint_library:Molex_Pico-Clasp_501331-0807_1x08-1MP_P1.00mm_Vertical</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>https://www.mouser.jp/ProductDetail/Molex/501331-0807?qs=uEWtSLL707WCWoLr2aeFsQ%3D%3D&amp;utm_source=OEMSecrets&amp;utm_medium=aggregator&amp;utm_campaign=5013310807&amp;utm_term=5013310807&amp;utm_content=Molex</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -272,10 +231,6 @@
   </si>
   <si>
     <t>https://www.mouser.jp/ProductDetail/Molex/501330-0400?qs=aXGKoampmnm6Ru8v6Lp%2Frg%3D%3D&amp;utm_source=OEMSecrets&amp;utm_medium=aggregator&amp;utm_campaign=5013300400&amp;utm_term=5013300400&amp;utm_content=Molex</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Connector_PinHeader_2.54mm:PinHeader_1x10_P2.54mm_Vertical</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -782,6 +737,17 @@
   </si>
   <si>
     <t>https://www.monotaro.com/p/6729/8762/?t.q=67298762</t>
+  </si>
+  <si>
+    <t>メモ</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>九州大学</t>
+    <rPh sb="0" eb="4">
+      <t>キュウシュウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
   </si>
 </sst>
 </file>
@@ -1406,7 +1372,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1424,9 +1390,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1789,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E44" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="89" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1813,48 +1776,48 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="H2">
         <v>23</v>
@@ -1863,31 +1826,28 @@
         <f>D2*H2</f>
         <v>23</v>
       </c>
-      <c r="J2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="H3">
         <v>26</v>
@@ -1896,31 +1856,28 @@
         <f t="shared" ref="I3:I48" si="0">D3*H3</f>
         <v>104</v>
       </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="H4">
         <v>55</v>
@@ -1929,31 +1886,28 @@
         <f t="shared" si="0"/>
         <v>385</v>
       </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="H5">
         <v>102</v>
@@ -1962,31 +1916,28 @@
         <f t="shared" si="0"/>
         <v>306</v>
       </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="H6">
         <v>363</v>
@@ -1995,31 +1946,28 @@
         <f t="shared" si="0"/>
         <v>726</v>
       </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="H7">
         <v>124</v>
@@ -2028,31 +1976,28 @@
         <f t="shared" si="0"/>
         <v>124</v>
       </c>
-      <c r="J7" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="H8">
         <v>29</v>
@@ -2061,31 +2006,28 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="J8" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F9" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="H9">
         <v>24</v>
@@ -2094,31 +2036,28 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="J9" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="H10">
         <v>540</v>
@@ -2127,31 +2066,28 @@
         <f t="shared" si="0"/>
         <v>1080</v>
       </c>
-      <c r="J10" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="G11" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="H11">
         <v>49</v>
@@ -2160,31 +2096,28 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="J11" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H12">
         <v>71</v>
@@ -2193,31 +2126,28 @@
         <f t="shared" si="0"/>
         <v>213</v>
       </c>
-      <c r="J12" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D13">
         <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="F13" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="H13">
         <v>17</v>
@@ -2226,31 +2156,28 @@
         <f t="shared" si="0"/>
         <v>136</v>
       </c>
-      <c r="J13" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>10000</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D14">
         <v>6</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="G14" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="H14">
         <v>17</v>
@@ -2259,31 +2186,28 @@
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="J14" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>3900</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="H15" s="3">
         <v>63</v>
@@ -2292,31 +2216,28 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="J15" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>1800</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="H16" s="3">
         <v>91</v>
@@ -2325,31 +2246,28 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="J16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B17">
         <v>390</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D17">
         <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="H17" s="3">
         <v>71</v>
@@ -2358,31 +2276,28 @@
         <f t="shared" si="0"/>
         <v>568</v>
       </c>
-      <c r="J17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B18">
         <v>1000</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="H18" s="3">
         <v>17</v>
@@ -2391,31 +2306,28 @@
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="J18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>4</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="H19" s="3">
         <v>1450</v>
@@ -2424,31 +2336,28 @@
         <f t="shared" si="0"/>
         <v>5800</v>
       </c>
-      <c r="J19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D20">
         <v>4</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="H20" s="3">
         <v>92</v>
@@ -2458,27 +2367,27 @@
         <v>368</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="G21" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="H21" s="3">
         <v>18</v>
@@ -2488,33 +2397,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:9">
       <c r="I22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:9">
       <c r="I23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:9">
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D24">
         <v>3</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="G24" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="H24">
         <v>38</v>
@@ -2524,21 +2433,21 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:9">
       <c r="C25" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F25" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="G25" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="H25">
         <v>55</v>
@@ -2548,21 +2457,21 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:9">
       <c r="C26" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="G26" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="H26">
         <v>35</v>
@@ -2572,21 +2481,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:9">
       <c r="C27" s="2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F27" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="G27" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="H27">
         <v>86</v>
@@ -2596,21 +2505,21 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:9">
       <c r="C28" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D28">
         <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F28" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="G28" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="H28">
         <v>53</v>
@@ -2620,21 +2529,21 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:9">
       <c r="C29" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D29">
         <v>28</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="F29" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="G29" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="H29">
         <v>28</v>
@@ -2644,21 +2553,21 @@
         <v>784</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:9">
       <c r="C30" s="2" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="D30">
         <v>16</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="F30" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="G30" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="H30">
         <v>17</v>
@@ -2668,27 +2577,27 @@
         <v>272</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:9">
       <c r="I31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:9">
       <c r="C32" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="D32">
         <v>12</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="F32" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="G32" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="H32">
         <v>1323</v>
@@ -2698,21 +2607,21 @@
         <v>15876</v>
       </c>
     </row>
-    <row r="33" spans="3:9">
+    <row r="33" spans="3:10">
       <c r="C33" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="F33" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G33" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="H33">
         <v>2353</v>
@@ -2722,18 +2631,18 @@
         <v>4706</v>
       </c>
     </row>
-    <row r="34" spans="3:9">
+    <row r="34" spans="3:10">
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="F34" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G34" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="H34">
         <v>479</v>
@@ -2743,21 +2652,21 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="35" spans="3:9">
+    <row r="35" spans="3:10">
       <c r="C35" s="2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="F35" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="G35" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="H35">
         <v>2581</v>
@@ -2767,21 +2676,21 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="36" spans="3:9">
+    <row r="36" spans="3:10">
       <c r="C36" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="F36" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="G36" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="H36">
         <v>1838</v>
@@ -2791,36 +2700,36 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="37" spans="3:9">
+    <row r="37" spans="3:10">
       <c r="I37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:9">
+    <row r="38" spans="3:10">
       <c r="I38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:9">
+    <row r="39" spans="3:10">
       <c r="I39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:9">
+    <row r="40" spans="3:10">
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="F40" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="G40" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="H40">
         <v>7445</v>
@@ -2830,21 +2739,21 @@
         <v>7445</v>
       </c>
     </row>
-    <row r="41" spans="3:9">
+    <row r="41" spans="3:10">
       <c r="C41" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="F41" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="G41" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="H41">
         <v>3841</v>
@@ -2854,37 +2763,36 @@
         <v>3841</v>
       </c>
     </row>
-    <row r="42" spans="3:9">
-      <c r="H42" s="6"/>
+    <row r="42" spans="3:10">
       <c r="I42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:9">
+    <row r="43" spans="3:10">
       <c r="I43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:9">
+    <row r="44" spans="3:10">
       <c r="I44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:9">
+    <row r="45" spans="3:10">
       <c r="C45" s="2" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="D45">
         <v>3</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="F45" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="G45" s="5">
         <v>3273198</v>
@@ -2896,19 +2804,22 @@
         <f t="shared" si="0"/>
         <v>1968</v>
       </c>
-    </row>
-    <row r="46" spans="3:9">
+      <c r="J45" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10">
       <c r="C46" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="D46">
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="F46" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="G46" s="5">
         <v>3210499</v>
@@ -2920,46 +2831,58 @@
         <f t="shared" si="0"/>
         <v>2438</v>
       </c>
-    </row>
-    <row r="47" spans="3:9">
+      <c r="J46" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10">
       <c r="G47" s="5"/>
-    </row>
-    <row r="48" spans="3:9">
+      <c r="J47" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10">
       <c r="I48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="4:9">
+      <c r="J48" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10">
       <c r="D49">
         <v>2</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>198</v>
+      <c r="E49" s="6" t="s">
+        <v>184</v>
       </c>
       <c r="F49" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="G49" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="H49" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="I49">
         <v>1994</v>
       </c>
-    </row>
-    <row r="50" spans="4:9">
+      <c r="J49" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10">
       <c r="D50">
         <v>4</v>
       </c>
-      <c r="E50" s="7"/>
+      <c r="E50" s="6"/>
       <c r="F50" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="G50" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="H50">
         <v>110</v>
@@ -2968,17 +2891,20 @@
         <f>D50*H50</f>
         <v>440</v>
       </c>
-    </row>
-    <row r="51" spans="4:9">
+      <c r="J50" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10">
       <c r="D51">
         <v>4</v>
       </c>
-      <c r="E51" s="7"/>
+      <c r="E51" s="6"/>
       <c r="F51" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G51" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="H51">
         <v>30</v>
@@ -2987,17 +2913,20 @@
         <f t="shared" ref="I51:I56" si="1">D51*H51</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="52" spans="4:9">
+      <c r="J51" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10">
       <c r="D52">
         <v>12</v>
       </c>
-      <c r="E52" s="7"/>
+      <c r="E52" s="6"/>
       <c r="F52" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="G52" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="H52">
         <v>32</v>
@@ -3006,22 +2935,28 @@
         <f t="shared" si="1"/>
         <v>384</v>
       </c>
-    </row>
-    <row r="53" spans="4:9">
+      <c r="J52" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="4:10">
       <c r="I53">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="4:9">
+      <c r="J53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="4:10">
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="F54" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="H54">
         <v>3290</v>
@@ -3030,16 +2965,19 @@
         <f t="shared" si="1"/>
         <v>3290</v>
       </c>
-    </row>
-    <row r="55" spans="4:9">
+      <c r="J54" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="4:10">
       <c r="D55">
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="F55" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="H55">
         <v>1898</v>
@@ -3048,16 +2986,19 @@
         <f t="shared" si="1"/>
         <v>3796</v>
       </c>
-    </row>
-    <row r="56" spans="4:9">
+      <c r="J55" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="56" spans="4:10">
       <c r="D56">
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F56" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="H56">
         <v>399</v>
@@ -3066,10 +3007,13 @@
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
-    </row>
-    <row r="57" spans="4:9">
+      <c r="J56" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="57" spans="4:10">
       <c r="H57" s="4" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="I57" s="4">
         <f>SUM(I2:I56)</f>

</xml_diff>